<commit_message>
Nhat Quang + Ngoc Hoan
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang1/02.XuLyBH/XLBH2301_KimLong.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang1/02.XuLyBH/XLBH2301_KimLong.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>STT</t>
   </si>
@@ -235,6 +235,24 @@
   </si>
   <si>
     <t>0000000212</t>
+  </si>
+  <si>
+    <t>Thiết bị không nhận nhiệt độ</t>
+  </si>
+  <si>
+    <t>Đổi mới thiết bị</t>
+  </si>
+  <si>
+    <t>Không sửa chữa được</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Tùng</t>
   </si>
 </sst>
 </file>
@@ -661,6 +679,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -708,9 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,7 +1037,7 @@
   <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1051,43 +1069,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
       <c r="W1" s="45"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="78" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="78"/>
+      <c r="F2" s="79"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="51"/>
@@ -1132,58 +1150,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="74" t="s">
+      <c r="A4" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="80" t="s">
+      <c r="K4" s="75"/>
+      <c r="L4" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="M4" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="80" t="s">
+      <c r="N4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="80" t="s">
+      <c r="O4" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="85" t="s">
+      <c r="P4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="80" t="s">
+      <c r="Q4" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="80" t="s">
+      <c r="R4" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="87" t="s">
+      <c r="S4" s="88" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="74" t="s">
+      <c r="V4" s="75" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="46"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="66" t="s">
         <v>1</v>
       </c>
@@ -1214,17 +1232,17 @@
       <c r="K5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="87"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="88"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
       <c r="W5" s="46"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,16 +1267,24 @@
       <c r="I6" s="69"/>
       <c r="J6" s="70"/>
       <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
+      <c r="L6" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="70" t="s">
+        <v>69</v>
+      </c>
       <c r="N6" s="71"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="71"/>
+      <c r="O6" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" s="71" t="s">
+        <v>73</v>
+      </c>
       <c r="Q6" s="72"/>
       <c r="R6" s="64"/>
       <c r="S6" s="73"/>
       <c r="T6" s="67"/>
-      <c r="U6" s="82" t="s">
+      <c r="U6" s="83" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1277,7 +1303,7 @@
       <c r="D7" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="74" t="s">
         <v>67</v>
       </c>
       <c r="F7" s="64"/>
@@ -1288,16 +1314,24 @@
       <c r="I7" s="69"/>
       <c r="J7" s="70"/>
       <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
+      <c r="L7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="70" t="s">
+        <v>70</v>
+      </c>
       <c r="N7" s="71"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="71"/>
+      <c r="O7" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7" s="71" t="s">
+        <v>73</v>
+      </c>
       <c r="Q7" s="72"/>
       <c r="R7" s="64"/>
-      <c r="S7" s="3"/>
+      <c r="S7" s="73"/>
       <c r="T7" s="67"/>
-      <c r="U7" s="83"/>
+      <c r="U7" s="84"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1310,7 +1344,7 @@
       <c r="B8" s="68">
         <v>44937</v>
       </c>
-      <c r="C8" s="63"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="64" t="s">
         <v>57</v>
       </c>
@@ -1322,19 +1356,27 @@
         <v>66</v>
       </c>
       <c r="H8" s="64"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="3"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="71"/>
+      <c r="O8" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="P8" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="73"/>
       <c r="T8" s="67"/>
-      <c r="U8" s="83"/>
+      <c r="U8" s="84"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1363,7 +1405,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="67"/>
-      <c r="U9" s="83"/>
+      <c r="U9" s="84"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1434,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="67"/>
-      <c r="U10" s="83"/>
+      <c r="U10" s="84"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1421,7 +1463,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="67"/>
-      <c r="U11" s="83"/>
+      <c r="U11" s="84"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1492,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="67"/>
-      <c r="U12" s="82" t="s">
+      <c r="U12" s="83" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1481,7 +1523,7 @@
       <c r="R13" s="37"/>
       <c r="S13" s="3"/>
       <c r="T13" s="67"/>
-      <c r="U13" s="83"/>
+      <c r="U13" s="84"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1510,7 +1552,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="67"/>
-      <c r="U14" s="83"/>
+      <c r="U14" s="84"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1539,7 +1581,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="83"/>
+      <c r="U15" s="84"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1568,7 +1610,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="84"/>
+      <c r="U16" s="85"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2306,7 +2348,7 @@
       </c>
       <c r="V40" s="9">
         <f>COUNTIF($O$6:$O$51,"*DM*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W40" s="13"/>
     </row>
@@ -2338,7 +2380,7 @@
       </c>
       <c r="V41" s="9">
         <f>COUNTIF($O$6:$O$51,"*KS*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W41" s="13"/>
     </row>
@@ -2857,43 +2899,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
       <c r="W1" s="45"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="89" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="90"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -2938,58 +2980,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="74" t="s">
+      <c r="A4" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="80" t="s">
+      <c r="L4" s="75"/>
+      <c r="M4" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="80" t="s">
+      <c r="N4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="O4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="88" t="s">
+      <c r="P4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="Q4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="74" t="s">
+      <c r="R4" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="87" t="s">
+      <c r="S4" s="88" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="74" t="s">
+      <c r="V4" s="75" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="46"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="42" t="s">
         <v>1</v>
       </c>
@@ -3014,23 +3056,23 @@
       <c r="I5" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="74"/>
+      <c r="J5" s="75"/>
       <c r="K5" s="42" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="87"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="88"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
       <c r="W5" s="46"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3056,7 +3098,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="41"/>
-      <c r="U6" s="82" t="s">
+      <c r="U6" s="83" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3087,7 +3129,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="41"/>
-      <c r="U7" s="83"/>
+      <c r="U7" s="84"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3116,7 +3158,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="41"/>
-      <c r="U8" s="83"/>
+      <c r="U8" s="84"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3145,7 +3187,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="41"/>
-      <c r="U9" s="83"/>
+      <c r="U9" s="84"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3174,7 +3216,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="41"/>
-      <c r="U10" s="83"/>
+      <c r="U10" s="84"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3203,7 +3245,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="41"/>
-      <c r="U11" s="83"/>
+      <c r="U11" s="84"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3232,7 +3274,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="41"/>
-      <c r="U12" s="82" t="s">
+      <c r="U12" s="83" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3263,7 +3305,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="41"/>
-      <c r="U13" s="83"/>
+      <c r="U13" s="84"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3292,7 +3334,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="41"/>
-      <c r="U14" s="83"/>
+      <c r="U14" s="84"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -3321,7 +3363,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="83"/>
+      <c r="U15" s="84"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3350,7 +3392,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="84"/>
+      <c r="U16" s="85"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>

</xml_diff>